<commit_message>
trying to connect and print a question
</commit_message>
<xml_diff>
--- a/docs/Product Backlog.xlsx
+++ b/docs/Product Backlog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="17235" windowHeight="8265"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="17235" windowHeight="4800"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,6 +15,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$28</definedName>
   </definedNames>
   <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -979,8 +980,8 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1040,7 +1041,7 @@
         <v>999</v>
       </c>
       <c r="E3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1141,7 +1142,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>41</v>
       </c>
@@ -1169,7 +1170,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -1225,7 +1226,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>40</v>
       </c>
@@ -1239,7 +1240,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>43</v>
       </c>
@@ -1253,7 +1254,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>35</v>
       </c>
@@ -1267,7 +1268,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>36</v>
       </c>
@@ -1281,7 +1282,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>44</v>
       </c>
@@ -1295,7 +1296,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>61</v>
       </c>
@@ -1337,7 +1338,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>49</v>
       </c>
@@ -1351,7 +1352,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>16</v>
       </c>
@@ -1385,7 +1386,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
Groomed story with new idea on question labels
for better search results
</commit_message>
<xml_diff>
--- a/docs/Product Backlog.xlsx
+++ b/docs/Product Backlog.xlsx
@@ -15,7 +15,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$28</definedName>
   </definedNames>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -133,11 +132,6 @@
 Because I want quick</t>
   </si>
   <si>
-    <t>As an administrator
-I want every saved exercise and its questions to have labels of question-type and topic
-Because the user wants auto-generated tests</t>
-  </si>
-  <si>
     <t>As a user
 When auto-generating a test, I want to narrow potential questions by selecting a category, and then choose what labels to include and exclude, e.g. by (de)selecting related labels in a word cloud
 Because I don't want irrelevant questions</t>
@@ -196,105 +190,110 @@
     <t>Duplicate</t>
   </si>
   <si>
+    <t>PBI021</t>
+  </si>
+  <si>
+    <t>As a user (history teacher/student)
+I want to make timelines, the events of which are saved and labeled ('war', 'birth', 'France', 'independence', …) for database purposes; I also want to generate timelines from chosen labels which are then customisable; I also want to generate gap-filling exercises from my timelines
+Because teachers want easy customisable timelines, and students want to easily learn timelines</t>
+  </si>
+  <si>
+    <t>PBI023</t>
+  </si>
+  <si>
+    <t>PBI022</t>
+  </si>
+  <si>
+    <t>As a developer
+I want the html to be in the right place
+Because that seems like a good next step</t>
+  </si>
+  <si>
+    <t>PBI024</t>
+  </si>
+  <si>
+    <t>As a developer
+I want the test questions saved in the database
+Because that seems like a good next step</t>
+  </si>
+  <si>
+    <t>PBI025</t>
+  </si>
+  <si>
+    <t>As a developer
+I want to make and save a simple test
+Because that seems like a good next step</t>
+  </si>
+  <si>
     <t>As a user
-I don't want to add a label to every question (require topic? Auto-copy from exercise?)
-Because I want fast</t>
+I want to see prior results by logging in
+Because it's educational</t>
+  </si>
+  <si>
+    <t>As a user
+I want to inform my teacher (owner of test and/or follower) and the app if a question is irrelevant (and specify why with labels) and exclude it from result calculations (whether this can be done depends on owner of test)
+Because I don't want irrelevant questions and inaccurate results</t>
+  </si>
+  <si>
+    <t>As a user
+I want to follow other users' progress (results)
+Because I want to help others</t>
+  </si>
+  <si>
+    <t>PBI026</t>
+  </si>
+  <si>
+    <t>As a user
+I want learning paths that can be made, shared and taken
+Because it maps my progress and/or the progress of my students</t>
+  </si>
+  <si>
+    <t>PBI029</t>
+  </si>
+  <si>
+    <t>As a developer
+I want to be able to call a (random) question from the db
+Because I need to learn</t>
+  </si>
+  <si>
+    <t>PBI031</t>
+  </si>
+  <si>
+    <t>As a developer
+I want to answer a question and have it checked
+Because essential</t>
+  </si>
+  <si>
+    <t>Not so much a job</t>
+  </si>
+  <si>
+    <t>self-evident</t>
+  </si>
+  <si>
+    <t>As a developer
+I want the results saved
+Because that seems like a good next step</t>
+  </si>
+  <si>
+    <t>As a developer
+I want to be able to save a question to the db with a form
+Because I need to learn</t>
+  </si>
+  <si>
+    <t>As an administrator
+I want every saved exercise and its questions to have labels of question-type, topic and anything else that can enhance search results
+Because the user wants auto-generated tests</t>
   </si>
   <si>
     <t>As a user
 I don't want labels to be fixed
 Because I might think of topics of my own
-(distinguish between category and (optional) label?)</t>
-  </si>
-  <si>
-    <t>PBI021</t>
-  </si>
-  <si>
-    <t>As a user (history teacher/student)
-I want to make timelines, the events of which are saved and labeled ('war', 'birth', 'France', 'independence', …) for database purposes; I also want to generate timelines from chosen labels which are then customisable; I also want to generate gap-filling exercises from my timelines
-Because teachers want easy customisable timelines, and students want to easily learn timelines</t>
-  </si>
-  <si>
-    <t>PBI023</t>
-  </si>
-  <si>
-    <t>PBI022</t>
-  </si>
-  <si>
-    <t>As a developer
-I want the html to be in the right place
-Because that seems like a good next step</t>
-  </si>
-  <si>
-    <t>PBI024</t>
-  </si>
-  <si>
-    <t>As a developer
-I want the test questions saved in the database
-Because that seems like a good next step</t>
-  </si>
-  <si>
-    <t>PBI025</t>
-  </si>
-  <si>
-    <t>As a developer
-I want to make and save a simple test
-Because that seems like a good next step</t>
+(distinguish between category and (optional) label? Users use labels/folders to order their tests; the names of which are copied to the database for better search results)</t>
   </si>
   <si>
     <t>As a user
-I want to see prior results by logging in
-Because it's educational</t>
-  </si>
-  <si>
-    <t>As a user
-I want to inform my teacher (owner of test and/or follower) and the app if a question is irrelevant (and specify why with labels) and exclude it from result calculations (whether this can be done depends on owner of test)
-Because I don't want irrelevant questions and inaccurate results</t>
-  </si>
-  <si>
-    <t>As a user
-I want to follow other users' progress (results)
-Because I want to help others</t>
-  </si>
-  <si>
-    <t>PBI026</t>
-  </si>
-  <si>
-    <t>As a user
-I want learning paths that can be made, shared and taken
-Because it maps my progress and/or the progress of my students</t>
-  </si>
-  <si>
-    <t>PBI029</t>
-  </si>
-  <si>
-    <t>As a developer
-I want to be able to call a (random) question from the db
-Because I need to learn</t>
-  </si>
-  <si>
-    <t>PBI031</t>
-  </si>
-  <si>
-    <t>As a developer
-I want to answer a question and have it checked
-Because essential</t>
-  </si>
-  <si>
-    <t>Not so much a job</t>
-  </si>
-  <si>
-    <t>self-evident</t>
-  </si>
-  <si>
-    <t>As a developer
-I want the results saved
-Because that seems like a good next step</t>
-  </si>
-  <si>
-    <t>As a developer
-I want to be able to save a question to the db with a form
-Because I need to learn</t>
+I don't want to add a label to every question (require topic? Copy folder names etc to database labels)
+Because I want fast</t>
   </si>
 </sst>
 </file>
@@ -980,8 +979,8 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1010,7 +1009,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1032,10 +1031,10 @@
     </row>
     <row r="3" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C3" s="4">
         <v>999</v>
@@ -1046,10 +1045,10 @@
     </row>
     <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C4" s="4">
         <v>999</v>
@@ -1060,10 +1059,10 @@
     </row>
     <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C5" s="4">
         <v>999</v>
@@ -1074,10 +1073,10 @@
     </row>
     <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C6" s="4">
         <v>997</v>
@@ -1088,10 +1087,10 @@
     </row>
     <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C7" s="4">
         <v>995</v>
@@ -1102,7 +1101,7 @@
     </row>
     <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>23</v>
@@ -1114,54 +1113,54 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>28</v>
+        <v>68</v>
       </c>
       <c r="C9" s="4">
         <v>900</v>
       </c>
       <c r="E9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="C10" s="4">
         <v>900</v>
       </c>
       <c r="E10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>48</v>
+        <v>69</v>
       </c>
       <c r="C11" s="4">
         <v>900</v>
       </c>
       <c r="E11" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C12" s="4">
         <v>900</v>
@@ -1172,10 +1171,10 @@
     </row>
     <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C13" s="4">
         <v>860</v>
@@ -1186,7 +1185,7 @@
     </row>
     <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>20</v>
@@ -1214,7 +1213,7 @@
     </row>
     <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>24</v>
@@ -1228,7 +1227,7 @@
     </row>
     <row r="17" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>25</v>
@@ -1242,10 +1241,10 @@
     </row>
     <row r="18" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C18" s="4">
         <v>700</v>
@@ -1256,7 +1255,7 @@
     </row>
     <row r="19" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>27</v>
@@ -1270,7 +1269,7 @@
     </row>
     <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>26</v>
@@ -1284,10 +1283,10 @@
     </row>
     <row r="21" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C21" s="4">
         <v>600</v>
@@ -1298,10 +1297,10 @@
     </row>
     <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C22" s="4">
         <v>500</v>
@@ -1340,10 +1339,10 @@
     </row>
     <row r="25" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C25" s="4">
         <v>100</v>
@@ -1366,15 +1365,15 @@
         <v>8</v>
       </c>
       <c r="F26" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C27" s="4">
         <v>0</v>
@@ -1383,7 +1382,7 @@
         <v>8</v>
       </c>
       <c r="F27" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="60" x14ac:dyDescent="0.25">
@@ -1400,15 +1399,15 @@
         <v>8</v>
       </c>
       <c r="F28" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C29" s="4">
         <v>0</v>
@@ -1419,10 +1418,10 @@
     </row>
     <row r="30" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C30" s="4">
         <v>0</v>
@@ -1431,7 +1430,7 @@
         <v>9</v>
       </c>
       <c r="F30" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Story marked as done
</commit_message>
<xml_diff>
--- a/docs/Product Backlog.xlsx
+++ b/docs/Product Backlog.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="17235" windowHeight="4800"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19140" windowHeight="7125"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,6 +15,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$28</definedName>
   </definedNames>
   <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -685,6 +686,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -732,7 +736,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -767,7 +771,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -979,8 +983,8 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1034,21 +1038,21 @@
         <v>60</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="C3" s="4">
         <v>999</v>
       </c>
       <c r="E3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C4" s="4">
         <v>999</v>
@@ -1059,13 +1063,13 @@
     </row>
     <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="C5" s="4">
-        <v>999</v>
+        <v>997</v>
       </c>
       <c r="E5" t="s">
         <v>5</v>
@@ -1073,13 +1077,13 @@
     </row>
     <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="C6" s="4">
-        <v>997</v>
+        <v>995</v>
       </c>
       <c r="E6" t="s">
         <v>5</v>
@@ -1087,13 +1091,13 @@
     </row>
     <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>66</v>
+        <v>23</v>
       </c>
       <c r="C7" s="4">
-        <v>995</v>
+        <v>910</v>
       </c>
       <c r="E7" t="s">
         <v>5</v>
@@ -1101,24 +1105,24 @@
     </row>
     <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>23</v>
+        <v>68</v>
       </c>
       <c r="C8" s="4">
-        <v>910</v>
+        <v>900</v>
       </c>
       <c r="E8" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C9" s="4">
         <v>900</v>
@@ -1129,10 +1133,10 @@
     </row>
     <row r="10" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C10" s="4">
         <v>900</v>
@@ -1143,27 +1147,27 @@
     </row>
     <row r="11" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>69</v>
+        <v>29</v>
       </c>
       <c r="C11" s="4">
         <v>900</v>
       </c>
       <c r="E11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>29</v>
+        <v>55</v>
       </c>
       <c r="C12" s="4">
-        <v>900</v>
+        <v>860</v>
       </c>
       <c r="E12" t="s">
         <v>5</v>
@@ -1171,13 +1175,13 @@
     </row>
     <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="C13" s="4">
-        <v>860</v>
+        <v>850</v>
       </c>
       <c r="E13" t="s">
         <v>5</v>
@@ -1185,13 +1189,13 @@
     </row>
     <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C14" s="4">
-        <v>850</v>
+        <v>720</v>
       </c>
       <c r="E14" t="s">
         <v>5</v>
@@ -1199,13 +1203,13 @@
     </row>
     <row r="15" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C15" s="4">
-        <v>720</v>
+        <v>700</v>
       </c>
       <c r="E15" t="s">
         <v>5</v>
@@ -1213,10 +1217,10 @@
     </row>
     <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C16" s="4">
         <v>700</v>
@@ -1227,10 +1231,10 @@
     </row>
     <row r="17" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C17" s="4">
         <v>700</v>
@@ -1241,13 +1245,13 @@
     </row>
     <row r="18" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C18" s="4">
-        <v>700</v>
+        <v>650</v>
       </c>
       <c r="E18" t="s">
         <v>5</v>
@@ -1255,10 +1259,10 @@
     </row>
     <row r="19" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C19" s="4">
         <v>650</v>
@@ -1269,13 +1273,13 @@
     </row>
     <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="C20" s="4">
-        <v>650</v>
+        <v>600</v>
       </c>
       <c r="E20" t="s">
         <v>5</v>
@@ -1283,13 +1287,13 @@
     </row>
     <row r="21" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C21" s="4">
-        <v>600</v>
+        <v>500</v>
       </c>
       <c r="E21" t="s">
         <v>5</v>
@@ -1297,13 +1301,13 @@
     </row>
     <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>58</v>
+        <v>14</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
       <c r="C22" s="4">
-        <v>500</v>
+        <v>410</v>
       </c>
       <c r="E22" t="s">
         <v>5</v>
@@ -1311,13 +1315,13 @@
     </row>
     <row r="23" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C23" s="4">
-        <v>410</v>
+        <v>400</v>
       </c>
       <c r="E23" t="s">
         <v>5</v>
@@ -1325,13 +1329,13 @@
     </row>
     <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="C24" s="4">
-        <v>400</v>
+        <v>100</v>
       </c>
       <c r="E24" t="s">
         <v>5</v>
@@ -1339,16 +1343,16 @@
     </row>
     <row r="25" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="C25" s="4">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="E25" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="45" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Backlog: added learning paths and youtube videos
</commit_message>
<xml_diff>
--- a/docs/Product Backlog.xlsx
+++ b/docs/Product Backlog.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="79">
   <si>
     <t>ID</t>
   </si>
@@ -290,11 +290,6 @@
 Because I want quick and simple</t>
   </si>
   <si>
-    <t>As a user
-I want to be able to save lessons and search lesson blocks by topic
-Because I want to easily browse and find the best material</t>
-  </si>
-  <si>
     <t>PBI033</t>
   </si>
   <si>
@@ -324,6 +319,19 @@
     <t>As a user
 I want multiple choice and other types of questions
 Because essential</t>
+  </si>
+  <si>
+    <t>PBI035</t>
+  </si>
+  <si>
+    <t>As a user
+I want customizable learning paths with youtube videos
+Because yay</t>
+  </si>
+  <si>
+    <t>As a user
+I want to be able to save lessons and search lesson blocks by topic
+Because I want to easily browse and find the best material to add to my learning paths</t>
   </si>
 </sst>
 </file>
@@ -385,7 +393,77 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="45">
+  <dxfs count="55">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF99CCFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCFF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF99CCFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCFF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1009,11 +1087,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1050,7 +1128,7 @@
         <v>52</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C2" s="4">
         <v>999</v>
@@ -1064,7 +1142,7 @@
         <v>67</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C3" s="4">
         <v>998</v>
@@ -1075,10 +1153,10 @@
     </row>
     <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>76</v>
       </c>
       <c r="C4" s="4">
         <v>996</v>
@@ -1087,7 +1165,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -1115,7 +1193,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>39</v>
       </c>
@@ -1129,7 +1207,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>40</v>
       </c>
@@ -1143,7 +1221,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -1171,7 +1249,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -1185,7 +1263,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>35</v>
       </c>
@@ -1199,7 +1277,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>38</v>
       </c>
@@ -1213,7 +1291,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>41</v>
       </c>
@@ -1227,7 +1305,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -1241,7 +1319,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -1255,7 +1333,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>42</v>
       </c>
@@ -1269,7 +1347,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>56</v>
       </c>
@@ -1313,44 +1391,44 @@
     </row>
     <row r="21" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>45</v>
+        <v>76</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
       <c r="C21" s="4">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E21" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="C22" s="4">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E22" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>72</v>
+        <v>46</v>
       </c>
       <c r="C23" s="4">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E23" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1440,7 +1518,7 @@
         <v>48</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C29" s="4">
         <v>0</v>
@@ -1508,9 +1586,23 @@
         <v>8</v>
       </c>
     </row>
+    <row r="34" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>60</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C34" s="4">
+        <v>0</v>
+      </c>
+      <c r="E34" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:F28">
-    <sortState ref="A2:F33">
+    <sortState ref="A2:F34">
       <sortCondition descending="1" ref="C1:C28"/>
     </sortState>
   </autoFilter>
@@ -1520,7 +1612,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="66" operator="equal" id="{CB7D9564-3487-49FA-8A45-F52788AC9C50}">
+          <x14:cfRule type="cellIs" priority="71" operator="equal" id="{CB7D9564-3487-49FA-8A45-F52788AC9C50}">
             <xm:f>Sheet2!$A$5</xm:f>
             <x14:dxf>
               <fill>
@@ -1530,7 +1622,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="67" operator="equal" id="{B5729598-715A-4761-B553-8527DF25944B}">
+          <x14:cfRule type="cellIs" priority="72" operator="equal" id="{B5729598-715A-4761-B553-8527DF25944B}">
             <xm:f>Sheet2!$A$4</xm:f>
             <x14:dxf>
               <fill>
@@ -1540,7 +1632,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="68" operator="equal" id="{FF39DD1E-B0DD-421A-84A2-8AB0E24F7209}">
+          <x14:cfRule type="cellIs" priority="73" operator="equal" id="{FF39DD1E-B0DD-421A-84A2-8AB0E24F7209}">
             <xm:f>Sheet2!$A$3</xm:f>
             <x14:dxf>
               <fill>
@@ -1550,7 +1642,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="69" operator="equal" id="{0ECD0148-6EB7-464B-9BCB-A9FC4B2151C7}">
+          <x14:cfRule type="cellIs" priority="74" operator="equal" id="{0ECD0148-6EB7-464B-9BCB-A9FC4B2151C7}">
             <xm:f>Sheet2!$A$2</xm:f>
             <x14:dxf>
               <fill>
@@ -1560,7 +1652,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="70" operator="equal" id="{E4D9DBE0-98C8-4F32-8943-840A9F89883A}">
+          <x14:cfRule type="cellIs" priority="75" operator="equal" id="{E4D9DBE0-98C8-4F32-8943-840A9F89883A}">
             <xm:f>Sheet2!$A$1</xm:f>
             <x14:dxf>
               <fill>
@@ -1570,10 +1662,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E1:E4 E22:E1048576</xm:sqref>
+          <xm:sqref>E1:E4 E22:E33 E35:E1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="51" operator="equal" id="{316265FB-6F61-4E57-B072-9D13F88053A6}">
+          <x14:cfRule type="cellIs" priority="56" operator="equal" id="{316265FB-6F61-4E57-B072-9D13F88053A6}">
             <xm:f>Sheet2!$A$5</xm:f>
             <x14:dxf>
               <fill>
@@ -1583,7 +1675,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="52" operator="equal" id="{1558288C-F0C2-4E34-ABBF-61B2143741AE}">
+          <x14:cfRule type="cellIs" priority="57" operator="equal" id="{1558288C-F0C2-4E34-ABBF-61B2143741AE}">
             <xm:f>Sheet2!$A$4</xm:f>
             <x14:dxf>
               <fill>
@@ -1593,7 +1685,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="53" operator="equal" id="{8509BF37-5861-4455-B8D2-8B585CDE3E42}">
+          <x14:cfRule type="cellIs" priority="58" operator="equal" id="{8509BF37-5861-4455-B8D2-8B585CDE3E42}">
             <xm:f>Sheet2!$A$3</xm:f>
             <x14:dxf>
               <fill>
@@ -1603,7 +1695,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="54" operator="equal" id="{591F26F2-DDDD-4086-93F0-7FAA449A5740}">
+          <x14:cfRule type="cellIs" priority="59" operator="equal" id="{591F26F2-DDDD-4086-93F0-7FAA449A5740}">
             <xm:f>Sheet2!$A$2</xm:f>
             <x14:dxf>
               <fill>
@@ -1613,7 +1705,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="55" operator="equal" id="{A9514637-DC0D-4B79-B668-6D80531E6E49}">
+          <x14:cfRule type="cellIs" priority="60" operator="equal" id="{A9514637-DC0D-4B79-B668-6D80531E6E49}">
             <xm:f>Sheet2!$A$1</xm:f>
             <x14:dxf>
               <fill>
@@ -1626,7 +1718,7 @@
           <xm:sqref>E5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="46" operator="equal" id="{CC2A681F-43BA-4F11-87CA-34E3F546E686}">
+          <x14:cfRule type="cellIs" priority="51" operator="equal" id="{CC2A681F-43BA-4F11-87CA-34E3F546E686}">
             <xm:f>Sheet2!$A$5</xm:f>
             <x14:dxf>
               <fill>
@@ -1636,7 +1728,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="47" operator="equal" id="{0BFAB624-CA97-4CE1-BBB6-A790385511BA}">
+          <x14:cfRule type="cellIs" priority="52" operator="equal" id="{0BFAB624-CA97-4CE1-BBB6-A790385511BA}">
             <xm:f>Sheet2!$A$4</xm:f>
             <x14:dxf>
               <fill>
@@ -1646,7 +1738,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="48" operator="equal" id="{8405E1A5-35B6-4998-BEA9-A3309E9D0C2F}">
+          <x14:cfRule type="cellIs" priority="53" operator="equal" id="{8405E1A5-35B6-4998-BEA9-A3309E9D0C2F}">
             <xm:f>Sheet2!$A$3</xm:f>
             <x14:dxf>
               <fill>
@@ -1656,7 +1748,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="49" operator="equal" id="{2BB4E676-0A98-4B16-A923-05DB0E325C6C}">
+          <x14:cfRule type="cellIs" priority="54" operator="equal" id="{2BB4E676-0A98-4B16-A923-05DB0E325C6C}">
             <xm:f>Sheet2!$A$2</xm:f>
             <x14:dxf>
               <fill>
@@ -1666,7 +1758,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="50" operator="equal" id="{B4A1B4E9-C44B-4664-8AC1-766C9919FD22}">
+          <x14:cfRule type="cellIs" priority="55" operator="equal" id="{B4A1B4E9-C44B-4664-8AC1-766C9919FD22}">
             <xm:f>Sheet2!$A$1</xm:f>
             <x14:dxf>
               <fill>
@@ -1679,7 +1771,7 @@
           <xm:sqref>E6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="41" operator="equal" id="{C8E68F9D-5E5F-4DCB-8724-98AE2EE0D07A}">
+          <x14:cfRule type="cellIs" priority="46" operator="equal" id="{C8E68F9D-5E5F-4DCB-8724-98AE2EE0D07A}">
             <xm:f>Sheet2!$A$5</xm:f>
             <x14:dxf>
               <fill>
@@ -1689,7 +1781,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="42" operator="equal" id="{E9191E40-6E4A-4900-AC66-F54C7E9B512D}">
+          <x14:cfRule type="cellIs" priority="47" operator="equal" id="{E9191E40-6E4A-4900-AC66-F54C7E9B512D}">
             <xm:f>Sheet2!$A$4</xm:f>
             <x14:dxf>
               <fill>
@@ -1699,7 +1791,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="43" operator="equal" id="{85611D12-A62A-4E4A-A181-6D56C7008841}">
+          <x14:cfRule type="cellIs" priority="48" operator="equal" id="{85611D12-A62A-4E4A-A181-6D56C7008841}">
             <xm:f>Sheet2!$A$3</xm:f>
             <x14:dxf>
               <fill>
@@ -1709,7 +1801,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="44" operator="equal" id="{CFF2874B-A7F8-45A8-BC59-67407FC781D6}">
+          <x14:cfRule type="cellIs" priority="49" operator="equal" id="{CFF2874B-A7F8-45A8-BC59-67407FC781D6}">
             <xm:f>Sheet2!$A$2</xm:f>
             <x14:dxf>
               <fill>
@@ -1719,7 +1811,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="45" operator="equal" id="{18089C4E-4068-49D0-9246-F8D5466C4818}">
+          <x14:cfRule type="cellIs" priority="50" operator="equal" id="{18089C4E-4068-49D0-9246-F8D5466C4818}">
             <xm:f>Sheet2!$A$1</xm:f>
             <x14:dxf>
               <fill>
@@ -1732,7 +1824,7 @@
           <xm:sqref>E7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="36" operator="equal" id="{EFCE2500-9847-456B-9F9D-CB72DF203080}">
+          <x14:cfRule type="cellIs" priority="41" operator="equal" id="{EFCE2500-9847-456B-9F9D-CB72DF203080}">
             <xm:f>Sheet2!$A$5</xm:f>
             <x14:dxf>
               <fill>
@@ -1742,7 +1834,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="37" operator="equal" id="{363D0CC2-F3F9-4B4E-B6FC-A6FA3F2A6E4D}">
+          <x14:cfRule type="cellIs" priority="42" operator="equal" id="{363D0CC2-F3F9-4B4E-B6FC-A6FA3F2A6E4D}">
             <xm:f>Sheet2!$A$4</xm:f>
             <x14:dxf>
               <fill>
@@ -1752,7 +1844,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="38" operator="equal" id="{2A92E722-2923-4FA5-8BEA-BD84C04D1E53}">
+          <x14:cfRule type="cellIs" priority="43" operator="equal" id="{2A92E722-2923-4FA5-8BEA-BD84C04D1E53}">
             <xm:f>Sheet2!$A$3</xm:f>
             <x14:dxf>
               <fill>
@@ -1762,7 +1854,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="39" operator="equal" id="{B29EA91E-6173-4956-9D6F-C8A3704B8B37}">
+          <x14:cfRule type="cellIs" priority="44" operator="equal" id="{B29EA91E-6173-4956-9D6F-C8A3704B8B37}">
             <xm:f>Sheet2!$A$2</xm:f>
             <x14:dxf>
               <fill>
@@ -1772,7 +1864,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="40" operator="equal" id="{151617BA-4968-480A-AC90-DCCA8F0A7DB0}">
+          <x14:cfRule type="cellIs" priority="45" operator="equal" id="{151617BA-4968-480A-AC90-DCCA8F0A7DB0}">
             <xm:f>Sheet2!$A$1</xm:f>
             <x14:dxf>
               <fill>
@@ -1785,7 +1877,7 @@
           <xm:sqref>E8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="31" operator="equal" id="{38A5808A-B7F2-4A78-92A7-8D174EC95405}">
+          <x14:cfRule type="cellIs" priority="36" operator="equal" id="{38A5808A-B7F2-4A78-92A7-8D174EC95405}">
             <xm:f>Sheet2!$A$5</xm:f>
             <x14:dxf>
               <fill>
@@ -1795,7 +1887,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="32" operator="equal" id="{1DBF5D8F-927B-4FE5-9CDF-6846808B013F}">
+          <x14:cfRule type="cellIs" priority="37" operator="equal" id="{1DBF5D8F-927B-4FE5-9CDF-6846808B013F}">
             <xm:f>Sheet2!$A$4</xm:f>
             <x14:dxf>
               <fill>
@@ -1805,7 +1897,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="33" operator="equal" id="{2B562433-E7AE-4782-8C37-47B9641BCA6B}">
+          <x14:cfRule type="cellIs" priority="38" operator="equal" id="{2B562433-E7AE-4782-8C37-47B9641BCA6B}">
             <xm:f>Sheet2!$A$3</xm:f>
             <x14:dxf>
               <fill>
@@ -1815,7 +1907,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="34" operator="equal" id="{1C58D6C8-7250-44EE-8F89-AB3F738C2F3C}">
+          <x14:cfRule type="cellIs" priority="39" operator="equal" id="{1C58D6C8-7250-44EE-8F89-AB3F738C2F3C}">
             <xm:f>Sheet2!$A$2</xm:f>
             <x14:dxf>
               <fill>
@@ -1825,7 +1917,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="35" operator="equal" id="{BE2DA3C3-9858-4EC3-A2C2-50F956FBAA76}">
+          <x14:cfRule type="cellIs" priority="40" operator="equal" id="{BE2DA3C3-9858-4EC3-A2C2-50F956FBAA76}">
             <xm:f>Sheet2!$A$1</xm:f>
             <x14:dxf>
               <fill>
@@ -1838,7 +1930,7 @@
           <xm:sqref>E9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="26" operator="equal" id="{49524AA4-9C3A-4B50-8028-6B46B87FF2CF}">
+          <x14:cfRule type="cellIs" priority="31" operator="equal" id="{49524AA4-9C3A-4B50-8028-6B46B87FF2CF}">
             <xm:f>Sheet2!$A$5</xm:f>
             <x14:dxf>
               <fill>
@@ -1848,7 +1940,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="27" operator="equal" id="{319E4111-D5C7-484F-84D5-24909304BEE1}">
+          <x14:cfRule type="cellIs" priority="32" operator="equal" id="{319E4111-D5C7-484F-84D5-24909304BEE1}">
             <xm:f>Sheet2!$A$4</xm:f>
             <x14:dxf>
               <fill>
@@ -1858,7 +1950,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="28" operator="equal" id="{3DA2F25E-D629-4085-9AE4-EC83A35F29ED}">
+          <x14:cfRule type="cellIs" priority="33" operator="equal" id="{3DA2F25E-D629-4085-9AE4-EC83A35F29ED}">
             <xm:f>Sheet2!$A$3</xm:f>
             <x14:dxf>
               <fill>
@@ -1868,7 +1960,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="29" operator="equal" id="{69E685A1-20C0-47B2-8B20-61EA20FEDC47}">
+          <x14:cfRule type="cellIs" priority="34" operator="equal" id="{69E685A1-20C0-47B2-8B20-61EA20FEDC47}">
             <xm:f>Sheet2!$A$2</xm:f>
             <x14:dxf>
               <fill>
@@ -1878,7 +1970,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="30" operator="equal" id="{B2D78BD4-E1D4-4172-9B14-B3E0A6031F20}">
+          <x14:cfRule type="cellIs" priority="35" operator="equal" id="{B2D78BD4-E1D4-4172-9B14-B3E0A6031F20}">
             <xm:f>Sheet2!$A$1</xm:f>
             <x14:dxf>
               <fill>
@@ -1891,7 +1983,7 @@
           <xm:sqref>E10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="21" operator="equal" id="{5E8A4EFE-E3D0-4BA8-AEF0-0FB6941C4F84}">
+          <x14:cfRule type="cellIs" priority="26" operator="equal" id="{5E8A4EFE-E3D0-4BA8-AEF0-0FB6941C4F84}">
             <xm:f>Sheet2!$A$5</xm:f>
             <x14:dxf>
               <fill>
@@ -1901,7 +1993,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="22" operator="equal" id="{2670F995-F26B-4329-AA93-6131CDAF15C2}">
+          <x14:cfRule type="cellIs" priority="27" operator="equal" id="{2670F995-F26B-4329-AA93-6131CDAF15C2}">
             <xm:f>Sheet2!$A$4</xm:f>
             <x14:dxf>
               <fill>
@@ -1911,7 +2003,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="23" operator="equal" id="{DE5194DA-5F23-43DE-8835-34C5692C2CD2}">
+          <x14:cfRule type="cellIs" priority="28" operator="equal" id="{DE5194DA-5F23-43DE-8835-34C5692C2CD2}">
             <xm:f>Sheet2!$A$3</xm:f>
             <x14:dxf>
               <fill>
@@ -1921,7 +2013,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="24" operator="equal" id="{C217A70E-20E8-4C2C-815F-6F97F5C5E1FD}">
+          <x14:cfRule type="cellIs" priority="29" operator="equal" id="{C217A70E-20E8-4C2C-815F-6F97F5C5E1FD}">
             <xm:f>Sheet2!$A$2</xm:f>
             <x14:dxf>
               <fill>
@@ -1931,7 +2023,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="25" operator="equal" id="{0B892F49-DC03-446F-9958-13DBFAB77338}">
+          <x14:cfRule type="cellIs" priority="30" operator="equal" id="{0B892F49-DC03-446F-9958-13DBFAB77338}">
             <xm:f>Sheet2!$A$1</xm:f>
             <x14:dxf>
               <fill>
@@ -1944,7 +2036,7 @@
           <xm:sqref>E11</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="1" operator="equal" id="{2C0AC945-E11D-47CC-893C-C9E13564A94E}">
+          <x14:cfRule type="cellIs" priority="6" operator="equal" id="{2C0AC945-E11D-47CC-893C-C9E13564A94E}">
             <xm:f>Sheet2!$A$5</xm:f>
             <x14:dxf>
               <fill>
@@ -1954,7 +2046,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="2" operator="equal" id="{65C86146-03B7-4FB1-8B92-CF5379ADB6E4}">
+          <x14:cfRule type="cellIs" priority="7" operator="equal" id="{65C86146-03B7-4FB1-8B92-CF5379ADB6E4}">
             <xm:f>Sheet2!$A$4</xm:f>
             <x14:dxf>
               <fill>
@@ -1964,7 +2056,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="3" operator="equal" id="{E3B3125B-A9FA-4A66-ABBB-EAF7E8C2D994}">
+          <x14:cfRule type="cellIs" priority="8" operator="equal" id="{E3B3125B-A9FA-4A66-ABBB-EAF7E8C2D994}">
             <xm:f>Sheet2!$A$3</xm:f>
             <x14:dxf>
               <fill>
@@ -1974,7 +2066,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="4" operator="equal" id="{C74206EC-5419-46D0-870E-B83497FBD849}">
+          <x14:cfRule type="cellIs" priority="9" operator="equal" id="{C74206EC-5419-46D0-870E-B83497FBD849}">
             <xm:f>Sheet2!$A$2</xm:f>
             <x14:dxf>
               <fill>
@@ -1984,7 +2076,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="5" operator="equal" id="{117BB76F-5818-423C-B424-AD5521DF8F2F}">
+          <x14:cfRule type="cellIs" priority="10" operator="equal" id="{117BB76F-5818-423C-B424-AD5521DF8F2F}">
             <xm:f>Sheet2!$A$1</xm:f>
             <x14:dxf>
               <fill>
@@ -1995,6 +2087,59 @@
             </x14:dxf>
           </x14:cfRule>
           <xm:sqref>E12:E21</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="1" operator="equal" id="{431CDB4C-6945-4DD5-A6AD-E67E8BF0240E}">
+            <xm:f>Sheet2!$A$5</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFFFFF"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="cellIs" priority="2" operator="equal" id="{68EE0BC4-D929-4300-8F47-916ED2A61DD4}">
+            <xm:f>Sheet2!$A$4</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFCCFF99"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="cellIs" priority="3" operator="equal" id="{2CCEAA3F-139D-4B96-8C75-B1FED9D7DD59}">
+            <xm:f>Sheet2!$A$3</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFFF99"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="cellIs" priority="4" operator="equal" id="{76E5CFA1-1F44-41DD-B423-1A6899FCD5AF}">
+            <xm:f>Sheet2!$A$2</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="9" tint="0.59996337778862885"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="cellIs" priority="5" operator="equal" id="{D2485745-9831-41E3-944E-11D49D8F910B}">
+            <xm:f>Sheet2!$A$1</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF99CCFF"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>E34</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
Backlog update: Prasso now saves results.
</commit_message>
<xml_diff>
--- a/docs/Product Backlog.xlsx
+++ b/docs/Product Backlog.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\docent\Documents\xampp\htdocs\Prasso\docs\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19140" windowHeight="7125"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="17850" windowHeight="10110"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,6 +15,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$28</definedName>
   </definedNames>
   <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -391,44 +387,9 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="55">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99CCFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="50">
     <dxf>
       <fill>
         <patternFill>
@@ -801,9 +762,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Kantoor">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -841,9 +802,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Kantoor">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -878,7 +839,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -913,7 +874,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Kantoor">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1091,7 +1052,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1125,13 +1086,13 @@
     </row>
     <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C2" s="4">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="E2" t="s">
         <v>5</v>
@@ -1139,13 +1100,13 @@
     </row>
     <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="C3" s="4">
-        <v>998</v>
+        <v>996</v>
       </c>
       <c r="E3" t="s">
         <v>5</v>
@@ -1153,24 +1114,24 @@
     </row>
     <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>74</v>
+        <v>36</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="C4" s="4">
-        <v>996</v>
+        <v>900</v>
       </c>
       <c r="E4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C5" s="4">
         <v>900</v>
@@ -1181,10 +1142,10 @@
     </row>
     <row r="6" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C6" s="4">
         <v>900</v>
@@ -1195,27 +1156,27 @@
     </row>
     <row r="7" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>65</v>
+        <v>28</v>
       </c>
       <c r="C7" s="4">
         <v>900</v>
       </c>
       <c r="E7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>28</v>
+        <v>53</v>
       </c>
       <c r="C8" s="4">
-        <v>900</v>
+        <v>860</v>
       </c>
       <c r="E8" t="s">
         <v>5</v>
@@ -1223,13 +1184,13 @@
     </row>
     <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>53</v>
+        <v>20</v>
       </c>
       <c r="C9" s="4">
-        <v>860</v>
+        <v>850</v>
       </c>
       <c r="E9" t="s">
         <v>5</v>
@@ -1237,13 +1198,13 @@
     </row>
     <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>20</v>
+        <v>68</v>
       </c>
       <c r="C10" s="4">
-        <v>850</v>
+        <v>720</v>
       </c>
       <c r="E10" t="s">
         <v>5</v>
@@ -1251,13 +1212,13 @@
     </row>
     <row r="11" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>68</v>
+        <v>23</v>
       </c>
       <c r="C11" s="4">
-        <v>720</v>
+        <v>700</v>
       </c>
       <c r="E11" t="s">
         <v>5</v>
@@ -1265,10 +1226,10 @@
     </row>
     <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C12" s="4">
         <v>700</v>
@@ -1279,10 +1240,10 @@
     </row>
     <row r="13" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C13" s="4">
         <v>700</v>
@@ -1293,13 +1254,13 @@
     </row>
     <row r="14" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C14" s="4">
-        <v>700</v>
+        <v>650</v>
       </c>
       <c r="E14" t="s">
         <v>5</v>
@@ -1307,10 +1268,10 @@
     </row>
     <row r="15" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C15" s="4">
         <v>650</v>
@@ -1321,13 +1282,13 @@
     </row>
     <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>25</v>
+        <v>54</v>
       </c>
       <c r="C16" s="4">
-        <v>650</v>
+        <v>600</v>
       </c>
       <c r="E16" t="s">
         <v>5</v>
@@ -1335,13 +1296,13 @@
     </row>
     <row r="17" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C17" s="4">
-        <v>600</v>
+        <v>500</v>
       </c>
       <c r="E17" t="s">
         <v>5</v>
@@ -1349,13 +1310,13 @@
     </row>
     <row r="18" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>56</v>
+        <v>14</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>57</v>
+        <v>21</v>
       </c>
       <c r="C18" s="4">
-        <v>500</v>
+        <v>410</v>
       </c>
       <c r="E18" t="s">
         <v>5</v>
@@ -1363,13 +1324,13 @@
     </row>
     <row r="19" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C19" s="4">
-        <v>410</v>
+        <v>400</v>
       </c>
       <c r="E19" t="s">
         <v>5</v>
@@ -1377,13 +1338,13 @@
     </row>
     <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>15</v>
+        <v>76</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>17</v>
+        <v>77</v>
       </c>
       <c r="C20" s="4">
-        <v>400</v>
+        <v>102</v>
       </c>
       <c r="E20" t="s">
         <v>5</v>
@@ -1391,13 +1352,13 @@
     </row>
     <row r="21" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C21" s="4">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E21" t="s">
         <v>5</v>
@@ -1405,13 +1366,13 @@
     </row>
     <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>69</v>
+        <v>45</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>78</v>
+        <v>46</v>
       </c>
       <c r="C22" s="4">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E22" t="s">
         <v>5</v>
@@ -1419,16 +1380,16 @@
     </row>
     <row r="23" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>46</v>
+        <v>73</v>
       </c>
       <c r="C23" s="4">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="E23" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1572,7 +1533,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>58</v>
       </c>
@@ -1586,7 +1547,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>60</v>
       </c>

</xml_diff>